<commit_message>
Excel file with timings for distributed version
</commit_message>
<xml_diff>
--- a/Prog4Dist.xlsx
+++ b/Prog4Dist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1639926\Documents\School_Stuff\FA2014\CSC410Par\Prog4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1954682\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -328,13 +328,13 @@
                   <c:v>17.492136199999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.037999999999998</c:v>
+                  <c:v>30.206137666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.086000000000002</c:v>
+                  <c:v>47.510750000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.187999999999999</c:v>
+                  <c:v>71.151401000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,7 +437,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>8 Threads</c:v>
+            <c:v>10 Threads</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -500,25 +500,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.186</c:v>
+                  <c:v>0.9209908</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3140000000000001</c:v>
+                  <c:v>2.8745538000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.54</c:v>
+                  <c:v>5.8527934000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1260000000000003</c:v>
+                  <c:v>9.9855467999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.3</c:v>
+                  <c:v>17.7077016</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.46</c:v>
+                  <c:v>24.071398000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.477999999999998</c:v>
+                  <c:v>35.332499999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -627,11 +627,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="300637712"/>
-        <c:axId val="300638104"/>
+        <c:axId val="206790032"/>
+        <c:axId val="206791664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="300637712"/>
+        <c:axId val="206790032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,7 +735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300638104"/>
+        <c:crossAx val="206791664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -744,7 +744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="300638104"/>
+        <c:axId val="206791664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,7 +856,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300637712"/>
+        <c:crossAx val="206790032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1189,13 +1189,13 @@
                   <c:v>2.0876438369679136</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2108738162485473</c:v>
+                  <c:v>2.0766805638055037</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2088342764329871</c:v>
+                  <c:v>2.0924908783801559</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2600112459202499</c:v>
+                  <c:v>2.0838549194554861</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1269,25 +1269,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.42584193548387</c:v>
+                  <c:v>2.5094784877329932</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0369385083713851</c:v>
+                  <c:v>2.7595716594345876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3023269491525431</c:v>
+                  <c:v>3.2070562066995225</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1245229207596594</c:v>
+                  <c:v>3.6570205983445327</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0998779674796744</c:v>
+                  <c:v>3.5424416119593971</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.108726156217883</c:v>
+                  <c:v>4.1300389366666614</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0298255309044038</c:v>
+                  <c:v>4.1963969999292434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1304,11 +1304,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="300638888"/>
-        <c:axId val="300639280"/>
+        <c:axId val="206792208"/>
+        <c:axId val="206792752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="300638888"/>
+        <c:axId val="206792208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,7 +1407,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300639280"/>
+        <c:crossAx val="206792752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1415,7 +1415,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="300639280"/>
+        <c:axId val="206792752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,7 +1522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300638888"/>
+        <c:crossAx val="206792208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1788,13 +1788,13 @@
                   <c:v>0.52191095924197839</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3027184540621368</c:v>
+                  <c:v>0.51917014095137592</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3022085691082468</c:v>
+                  <c:v>0.52312271959503898</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3150028114800625</c:v>
+                  <c:v>0.52096372986387152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1838,25 +1838,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.5532302419354838</c:v>
+                  <c:v>0.25094784877329934</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75461731354642314</c:v>
+                  <c:v>0.27595716594345876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66279086864406789</c:v>
+                  <c:v>0.32070562066995223</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64056536509495743</c:v>
+                  <c:v>0.36570205983445325</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6374847459349593</c:v>
+                  <c:v>0.35424416119593971</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.63859076952723537</c:v>
+                  <c:v>0.41300389366666612</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.62872819136305047</c:v>
+                  <c:v>0.41963969999292433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1873,11 +1873,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="300640064"/>
-        <c:axId val="300640456"/>
+        <c:axId val="248857936"/>
+        <c:axId val="248843792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="300640064"/>
+        <c:axId val="248857936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1976,7 +1976,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300640456"/>
+        <c:crossAx val="248843792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1984,7 +1984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="300640456"/>
+        <c:axId val="248843792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2091,7 +2091,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300640064"/>
+        <c:crossAx val="248857936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4129,8 +4129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4762,31 +4762,25 @@
         <v>4</v>
       </c>
       <c r="D20">
-        <v>12.03</v>
+        <v>30.251967</v>
       </c>
       <c r="E20">
-        <v>12.03</v>
+        <v>30.171503999999999</v>
       </c>
       <c r="F20">
-        <v>12.04</v>
-      </c>
-      <c r="G20">
-        <v>12.05</v>
-      </c>
-      <c r="H20">
-        <v>12.04</v>
+        <v>30.194942000000001</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="2"/>
-        <v>12.037999999999998</v>
+        <v>30.206137666666667</v>
       </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>5.2108738162485473</v>
+        <v>2.0766805638055037</v>
       </c>
       <c r="K20" s="3">
         <f t="shared" si="1"/>
-        <v>1.3027184540621368</v>
+        <v>0.51917014095137592</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -4798,31 +4792,22 @@
         <v>4</v>
       </c>
       <c r="D21">
-        <v>19.09</v>
+        <v>47.513663999999999</v>
       </c>
       <c r="E21">
-        <v>19.079999999999998</v>
-      </c>
-      <c r="F21">
-        <v>19.09</v>
-      </c>
-      <c r="G21">
-        <v>19.09</v>
-      </c>
-      <c r="H21">
-        <v>19.079999999999998</v>
+        <v>47.507835999999998</v>
       </c>
       <c r="I21" s="3">
         <f t="shared" si="2"/>
-        <v>19.086000000000002</v>
+        <v>47.510750000000002</v>
       </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>5.2088342764329871</v>
+        <v>2.0924908783801559</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" si="1"/>
-        <v>1.3022085691082468</v>
+        <v>0.52312271959503898</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -4834,31 +4819,19 @@
         <v>4</v>
       </c>
       <c r="D22">
-        <v>28.27</v>
-      </c>
-      <c r="E22">
-        <v>28.17</v>
-      </c>
-      <c r="F22">
-        <v>28.17</v>
-      </c>
-      <c r="G22">
-        <v>28.16</v>
-      </c>
-      <c r="H22">
-        <v>28.17</v>
+        <v>71.151401000000007</v>
       </c>
       <c r="I22" s="3">
         <f t="shared" si="2"/>
-        <v>28.187999999999999</v>
+        <v>71.151401000000007</v>
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>5.2600112459202499</v>
+        <v>2.0838549194554861</v>
       </c>
       <c r="K22" s="3">
         <f t="shared" si="1"/>
-        <v>1.3150028114800625</v>
+        <v>0.52096372986387152</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -4867,34 +4840,34 @@
         <v>1000</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D23">
-        <v>0.18</v>
+        <v>0.90959000000000001</v>
       </c>
       <c r="E23">
-        <v>0.19</v>
+        <v>0.91850600000000004</v>
       </c>
       <c r="F23">
-        <v>0.19</v>
+        <v>0.95283300000000004</v>
       </c>
       <c r="G23">
-        <v>0.18</v>
+        <v>0.90574699999999997</v>
       </c>
       <c r="H23">
-        <v>0.19</v>
+        <v>0.91827800000000004</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="2"/>
-        <v>0.186</v>
+        <v>0.9209908</v>
       </c>
       <c r="J23">
         <f>I2/I23</f>
-        <v>12.42584193548387</v>
+        <v>2.5094784877329932</v>
       </c>
       <c r="K23" s="3">
         <f t="shared" si="1"/>
-        <v>1.5532302419354838</v>
+        <v>0.25094784877329934</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -4903,34 +4876,34 @@
         <v>1500</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>1.31</v>
+        <v>2.8921329999999998</v>
       </c>
       <c r="E24">
-        <v>1.32</v>
+        <v>3.0182899999999999</v>
       </c>
       <c r="F24">
-        <v>1.32</v>
+        <v>2.7994430000000001</v>
       </c>
       <c r="G24">
-        <v>1.31</v>
+        <v>2.8246920000000002</v>
       </c>
       <c r="H24">
-        <v>1.31</v>
+        <v>2.8382109999999998</v>
       </c>
       <c r="I24" s="3">
         <f t="shared" si="2"/>
-        <v>1.3140000000000001</v>
+        <v>2.8745538000000002</v>
       </c>
       <c r="J24">
         <f t="shared" ref="J24:J29" si="5">I3/I24</f>
-        <v>6.0369385083713851</v>
+        <v>2.7595716594345876</v>
       </c>
       <c r="K24" s="3">
         <f t="shared" si="1"/>
-        <v>0.75461731354642314</v>
+        <v>0.27595716594345876</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -4939,34 +4912,34 @@
         <v>2000</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>3.55</v>
+        <v>5.7810620000000004</v>
       </c>
       <c r="E25">
-        <v>3.54</v>
+        <v>5.9899050000000003</v>
       </c>
       <c r="F25">
-        <v>3.54</v>
+        <v>5.7378309999999999</v>
       </c>
       <c r="G25">
-        <v>3.53</v>
+        <v>5.4690719999999997</v>
       </c>
       <c r="H25">
-        <v>3.54</v>
+        <v>6.2860969999999998</v>
       </c>
       <c r="I25" s="3">
         <f t="shared" si="2"/>
-        <v>3.54</v>
+        <v>5.8527934000000004</v>
       </c>
       <c r="J25">
         <f t="shared" si="5"/>
-        <v>5.3023269491525431</v>
+        <v>3.2070562066995225</v>
       </c>
       <c r="K25" s="3">
         <f t="shared" si="1"/>
-        <v>0.66279086864406789</v>
+        <v>0.32070562066995223</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -4975,34 +4948,34 @@
         <v>2500</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D26">
-        <v>7.11</v>
+        <v>9.8542629999999996</v>
       </c>
       <c r="E26">
-        <v>7.07</v>
+        <v>10.087362000000001</v>
       </c>
       <c r="F26">
-        <v>7.3</v>
+        <v>10.006361</v>
       </c>
       <c r="G26">
-        <v>7.07</v>
+        <v>10.208990999999999</v>
       </c>
       <c r="H26">
-        <v>7.08</v>
+        <v>9.7707569999999997</v>
       </c>
       <c r="I26" s="3">
         <f t="shared" si="2"/>
-        <v>7.1260000000000003</v>
+        <v>9.9855467999999998</v>
       </c>
       <c r="J26">
         <f t="shared" si="5"/>
-        <v>5.1245229207596594</v>
+        <v>3.6570205983445327</v>
       </c>
       <c r="K26" s="3">
         <f t="shared" si="1"/>
-        <v>0.64056536509495743</v>
+        <v>0.36570205983445325</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -5011,34 +4984,34 @@
         <v>3000</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D27">
-        <v>12.29</v>
+        <v>17.342290999999999</v>
       </c>
       <c r="E27">
-        <v>12.3</v>
+        <v>19.105416999999999</v>
       </c>
       <c r="F27">
-        <v>12.31</v>
+        <v>16.453430000000001</v>
       </c>
       <c r="G27">
-        <v>12.29</v>
+        <v>19.987310000000001</v>
       </c>
       <c r="H27">
-        <v>12.31</v>
+        <v>15.65006</v>
       </c>
       <c r="I27" s="3">
         <f t="shared" si="2"/>
-        <v>12.3</v>
+        <v>17.7077016</v>
       </c>
       <c r="J27">
         <f t="shared" si="5"/>
-        <v>5.0998779674796744</v>
+        <v>3.5424416119593971</v>
       </c>
       <c r="K27" s="3">
         <f t="shared" si="1"/>
-        <v>0.6374847459349593</v>
+        <v>0.35424416119593971</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -5047,34 +5020,34 @@
         <v>3500</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D28">
-        <v>19.48</v>
+        <v>23.859414999999998</v>
       </c>
       <c r="E28">
-        <v>19.3</v>
+        <v>23.655825</v>
       </c>
       <c r="F28">
-        <v>19.47</v>
+        <v>24.41619</v>
       </c>
       <c r="G28">
-        <v>19.579999999999998</v>
+        <v>24.504135999999999</v>
       </c>
       <c r="H28">
-        <v>19.47</v>
+        <v>23.921423999999998</v>
       </c>
       <c r="I28" s="3">
         <f t="shared" si="2"/>
-        <v>19.46</v>
+        <v>24.071398000000002</v>
       </c>
       <c r="J28">
         <f t="shared" si="5"/>
-        <v>5.108726156217883</v>
+        <v>4.1300389366666614</v>
       </c>
       <c r="K28" s="3">
         <f t="shared" si="1"/>
-        <v>0.63859076952723537</v>
+        <v>0.41300389366666612</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -5083,34 +5056,34 @@
         <v>4000</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D29">
-        <v>31.22</v>
+        <v>35.750883000000002</v>
       </c>
       <c r="E29">
-        <v>28.83</v>
+        <v>35.474902</v>
       </c>
       <c r="F29">
-        <v>28.83</v>
+        <v>34.902188000000002</v>
       </c>
       <c r="G29">
-        <v>29.25</v>
+        <v>34.638267999999997</v>
       </c>
       <c r="H29">
-        <v>29.26</v>
+        <v>35.896259000000001</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="2"/>
-        <v>29.477999999999998</v>
+        <v>35.332499999999996</v>
       </c>
       <c r="J29">
         <f t="shared" si="5"/>
-        <v>5.0298255309044038</v>
+        <v>4.1963969999292434</v>
       </c>
       <c r="K29" s="3">
         <f t="shared" si="1"/>
-        <v>0.62872819136305047</v>
+        <v>0.41963969999292433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Document ALL the things!
</commit_message>
<xml_diff>
--- a/Prog4Dist.xlsx
+++ b/Prog4Dist.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1954682\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="9675"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,26 +167,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -627,11 +602,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206790032"/>
-        <c:axId val="206791664"/>
+        <c:axId val="108926848"/>
+        <c:axId val="108941696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206790032"/>
+        <c:axId val="108926848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,26 +652,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -735,7 +690,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206791664"/>
+        <c:crossAx val="108941696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -744,7 +699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206791664"/>
+        <c:axId val="108941696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,26 +759,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -856,7 +791,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206790032"/>
+        <c:crossAx val="108926848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -991,26 +926,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1206,7 +1121,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>8 Threads</c:v>
+            <c:v>10 Threads</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1304,11 +1219,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206792208"/>
-        <c:axId val="206792752"/>
+        <c:axId val="109396736"/>
+        <c:axId val="109399040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206792208"/>
+        <c:axId val="109396736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,26 +1264,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1407,7 +1302,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206792752"/>
+        <c:crossAx val="109399040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1415,7 +1310,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206792752"/>
+        <c:axId val="109399040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,26 +1365,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1522,7 +1397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206792208"/>
+        <c:crossAx val="109396736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1534,6 +1409,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1620,26 +1500,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1805,7 +1665,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>8 Threads</c:v>
+            <c:v>10 Threads</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1873,11 +1733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="248857936"/>
-        <c:axId val="248843792"/>
+        <c:axId val="109437312"/>
+        <c:axId val="109439616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="248857936"/>
+        <c:axId val="109437312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,26 +1778,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1976,7 +1816,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248843792"/>
+        <c:crossAx val="109439616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1984,7 +1824,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="248843792"/>
+        <c:axId val="109439616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2039,26 +1879,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2091,7 +1911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248857936"/>
+        <c:crossAx val="109437312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2103,6 +1923,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4119,7 +3944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4129,8 +3954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="Y36" sqref="Y36"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>